<commit_message>
Rewrote preprocessing for better accounting of timings
*Exclusion criteria for cases start date of EHR sampling* (if restrict_to_event_period is True):
- EHR sampling start date needs to at most 10 days before stroke onset (so that 14 days periods includes 72h of stroke monitoring) [when stroke onset is not available, arrival date from registry is used]
- EHR sampling start date should be at most 7 days after reference date in registry (stroke onset or arrival date, whichever is later)
</commit_message>
<xml_diff>
--- a/preprocessing/variable_assembly/selected_variables.xlsx
+++ b/preprocessing/variable_assembly/selected_variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk1/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk1/stroke_research/OPSUM/preprocessing/variable_assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C69166-1EF2-9340-90A1-D249B7B4CA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9430B6BF-2064-1A4D-9CAD-3A716309809E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{4EF3017B-64DF-5142-A0B6-DCCDE5805A97}"/>
   </bookViews>
@@ -610,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68269D3-7424-0349-8C48-DE37DFBA5500}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,7 +676,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
@@ -692,256 +692,254 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reformated lab preprocessing for Extraction_20220815
</commit_message>
<xml_diff>
--- a/preprocessing/variable_assembly/selected_variables.xlsx
+++ b/preprocessing/variable_assembly/selected_variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk1/stroke_research/OPSUM/preprocessing/variable_assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12845672-D9B3-7244-9D4F-5B4918726FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08729430-D04A-1E4B-990D-9AD409ED3703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{4EF3017B-64DF-5142-A0B6-DCCDE5805A97}"/>
   </bookViews>
@@ -646,7 +646,7 @@
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
For patients without FiO2, fiO2 is inferred to 21% with sample date set to first sample date found in EHR
</commit_message>
<xml_diff>
--- a/preprocessing/variable_assembly/selected_variables.xlsx
+++ b/preprocessing/variable_assembly/selected_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk1/stroke_research/OPSUM/preprocessing/variable_assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08729430-D04A-1E4B-990D-9AD409ED3703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64555D7E-C87C-364C-9A26-BCBA3FBC971E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{4EF3017B-64DF-5142-A0B6-DCCDE5805A97}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>Activite anti-Xa (DOAC)</t>
   </si>
@@ -643,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68269D3-7424-0349-8C48-DE37DFBA5500}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -846,176 +846,171 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified french accent processing and enforced presence of all selected variables
all variables from the variable selection file must be present in the dataframe
</commit_message>
<xml_diff>
--- a/preprocessing/variable_assembly/selected_variables.xlsx
+++ b/preprocessing/variable_assembly/selected_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jk1/stroke_research/OPSUM/preprocessing/variable_assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64555D7E-C87C-364C-9A26-BCBA3FBC971E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04698EEA-0E75-EC45-AC7E-E2B18130788A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{4EF3017B-64DF-5142-A0B6-DCCDE5805A97}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{4EF3017B-64DF-5142-A0B6-DCCDE5805A97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Activite anti-Xa (DOAC)</t>
   </si>
@@ -181,9 +181,6 @@
     <t>Prestroke disability (Rankin)</t>
   </si>
   <si>
-    <t>NIH on admission</t>
-  </si>
-  <si>
     <t>Antihypert. drugs pre-stroke</t>
   </si>
   <si>
@@ -215,12 +212,6 @@
   </si>
   <si>
     <t>MedHist PAD</t>
-  </si>
-  <si>
-    <t>1st cholesterol total</t>
-  </si>
-  <si>
-    <t>1st cholesterol LDL</t>
   </si>
   <si>
     <t>MedHist cerebrovascular_event</t>
@@ -643,20 +634,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68269D3-7424-0349-8C48-DE37DFBA5500}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -669,7 +660,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -736,7 +727,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -744,7 +735,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -752,7 +743,7 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -760,7 +751,7 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -768,7 +759,7 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -776,242 +767,226 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>